<commit_message>
JD - removed unnecessary additions
</commit_message>
<xml_diff>
--- a/etc/Acceptance Test Plan.xlsx
+++ b/etc/Acceptance Test Plan.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>User Story</t>
   </si>
@@ -50,22 +50,7 @@
     <t>Given that I am on the products page when there are products in the inventory then I see a means to add each product to my shopping cart.</t>
   </si>
   <si>
-    <t>As an Admin I want to add new products to the inventory so that I can expand my business.</t>
-  </si>
-  <si>
-    <t>Given I am not an admin, when I view the website, then I will not see an option to add products.</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>JD; 10/16; I do not see an option to add products as a user</t>
-  </si>
-  <si>
-    <t>Given I am an admin, when I select the option to add a product to the inventory, with inputs for name, quantity, and price, then the product will be added.</t>
-  </si>
-  <si>
-    <t>JD; 10/16; I see an option to add products as an admin</t>
+    <t/>
   </si>
   <si>
     <t>Instructions</t>
@@ -96,7 +81,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +100,12 @@
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -167,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -184,10 +175,16 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -196,11 +193,17 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -513,36 +516,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="21.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="106.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="15" width="21.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="16" width="106.86214285714286" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="243.75">
-      <c r="A1" s="10" t="s">
-        <v>17</v>
+      <c r="A1" s="12" t="s">
+        <v>12</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="23.25">
-      <c r="A3" s="10" t="s">
-        <v>19</v>
+      <c r="A3" s="12" t="s">
+        <v>14</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>20</v>
+      <c r="B3" s="14" t="s">
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="23.25">
-      <c r="A4" s="10" t="s">
-        <v>21</v>
+      <c r="A4" s="12" t="s">
+        <v>16</v>
       </c>
-      <c r="B4" s="11" t="s">
-        <v>22</v>
+      <c r="B4" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -563,12 +566,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="30.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="60.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="60.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="60.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="30.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="60.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="60.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="60.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
@@ -613,7 +616,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A4" s="4"/>
       <c r="B4" s="4" t="s">
         <v>8</v>
@@ -623,7 +626,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="33.75" customFormat="1" s="1">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
@@ -633,7 +636,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="47.25" customFormat="1" s="1">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
@@ -643,37 +646,37 @@
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="48" customFormat="1" s="1">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>13</v>
+      <c r="C7" s="8" t="s">
+        <v>11</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>14</v>
+      <c r="D7" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="45.75" customFormat="1" s="1">
       <c r="A8" s="6"/>
-      <c r="B8" s="6" t="s">
-        <v>15</v>
+      <c r="B8" s="9" t="s">
+        <v>11</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>13</v>
+      <c r="C8" s="8" t="s">
+        <v>11</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>16</v>
+      <c r="D8" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="5"/>
@@ -681,7 +684,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="5"/>
@@ -689,7 +692,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="5"/>
@@ -697,7 +700,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="5"/>
@@ -705,7 +708,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="5"/>
@@ -713,7 +716,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="5"/>
@@ -721,7 +724,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
@@ -729,7 +732,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5"/>
@@ -737,7 +740,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5"/>
@@ -745,7 +748,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5"/>
@@ -753,7 +756,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="5"/>
@@ -761,7 +764,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="5"/>
@@ -769,7 +772,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25" customFormat="1" s="1">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="5"/>

</xml_diff>